<commit_message>
done up to and including bbr checks
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Value</t>
   </si>
@@ -52,9 +52,6 @@
     <t>PRT naming convention</t>
   </si>
   <si>
-    <t>PRT.FORMAT</t>
-  </si>
-  <si>
     <t>Perform linear trend removal</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
   </si>
   <si>
     <t>E:\Guy\PRTs</t>
-  </si>
-  <si>
-    <t>Leave empty if PRT are already in BV participant directories</t>
   </si>
   <si>
     <t>Can include wildcard (*). Will replace [P#], [R#], and/or [PID]. If numbers are forced to a min number of digits (e.g., forcing 2-digits yields 02 instead of 2), state the number of digits after the #-sign. For example, [R#2] will insert a 2-digit run number.</t>
@@ -216,6 +210,33 @@
       <t xml:space="preserve"> (supports both P1 and P01 formats - i.e., %0#d formats). 
 Example: "AB12, CD23" (AB12 is participant 1, CD23 is participant 2)</t>
     </r>
+  </si>
+  <si>
+    <t>PRT.NAMING</t>
+  </si>
+  <si>
+    <t>Anat</t>
+  </si>
+  <si>
+    <t>Function name</t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Anatomical name</t>
+  </si>
+  <si>
+    <t>VMR.NAME</t>
+  </si>
+  <si>
+    <t>VTC.NAME</t>
+  </si>
+  <si>
+    <t>Name entered in the Create Document Workflow.</t>
+  </si>
+  <si>
+    <t>Leave empty if PRT are already in BV participant directories. Will search BV directory before searching this directory.</t>
   </si>
 </sst>
 </file>
@@ -337,8 +358,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E30" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E32" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E32"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -637,24 +658,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="73.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
     <col min="4" max="4" width="74.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -671,13 +692,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -692,7 +713,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -701,16 +722,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -725,17 +746,17 @@
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -744,37 +765,43 @@
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="B8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="6">
-        <v>8</v>
+        <v>52</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,127 +811,137 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="6">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="6">
-        <v>2</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="6">
-        <v>3</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="6">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="6">
         <v>6</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="6"/>
       <c r="D16" s="5" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="B17" s="5"/>
       <c r="C17" s="6"/>
-      <c r="D17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="7"/>
+        <v>36</v>
+      </c>
+      <c r="C18" s="6"/>
       <c r="D18" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -975,6 +1012,20 @@
       <c r="C30" s="6"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
done up to and include MotionChecks
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Value</t>
   </si>
@@ -236,7 +236,22 @@
     <t>Name entered in the Create Document Workflow.</t>
   </si>
   <si>
+    <t>1-2</t>
+  </si>
+  <si>
     <t>Leave empty if PRT are already in BV participant directories. Will search BV directory before searching this directory.</t>
+  </si>
+  <si>
+    <t>Motion</t>
+  </si>
+  <si>
+    <t>MTN.OVERWRITE</t>
+  </si>
+  <si>
+    <t>Create motion plots even if already run (overwrites prior)</t>
+  </si>
+  <si>
+    <t>TRUE or FALSE. Set true to always generate new motion plots.</t>
   </si>
 </sst>
 </file>
@@ -660,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +746,7 @@
         <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -935,7 +950,9 @@
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="D20" s="5" t="s">
         <v>44</v>
       </c>
@@ -951,11 +968,21 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="A22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>

</xml_diff>

<commit_message>
switched to global p, finished LinkVTCtoPRT
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
completed up to and including CheckAndFinishVTCPreprocessing
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Value</t>
   </si>
@@ -52,21 +52,6 @@
     <t>PRT naming convention</t>
   </si>
   <si>
-    <t>Perform linear trend removal</t>
-  </si>
-  <si>
-    <t>TRUE or FALSE. Will not repeat if already performed.</t>
-  </si>
-  <si>
-    <t>Leave blank or set 0 to disable. Will not repeat if already performed.</t>
-  </si>
-  <si>
-    <t>VTC.LTR</t>
-  </si>
-  <si>
-    <t>VTC.THP</t>
-  </si>
-  <si>
     <t>VTC.SS</t>
   </si>
   <si>
@@ -152,12 +137,6 @@
   </si>
   <si>
     <t>Temporal high pass filter number of cycles (if included in fmr preprocessing)</t>
-  </si>
-  <si>
-    <t>If THP was run on FMR with a value other than this, an error will be thrown. Leave blank or set 0 to disable the check.</t>
-  </si>
-  <si>
-    <t>Leave blank or set 0 to disable. Will not repeat if already performed on fmr or vtc.</t>
   </si>
   <si>
     <t>PAR.RUN</t>
@@ -236,9 +215,6 @@
     <t>Name entered in the Create Document Workflow.</t>
   </si>
   <si>
-    <t>1-2</t>
-  </si>
-  <si>
     <t>Leave empty if PRT are already in BV participant directories. Will search BV directory before searching this directory.</t>
   </si>
   <si>
@@ -252,6 +228,63 @@
   </si>
   <si>
     <t>TRUE or FALSE. Set true to always generate new motion plots.</t>
+  </si>
+  <si>
+    <t>VTC.THP_FMR</t>
+  </si>
+  <si>
+    <t>VTC.THP_VTC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leave blank or set 0 to skip spatial smoothing. This will also skip MDM generation.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(TYPICAL VALUES: 6 or 8)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leave blank or set 0 if THP should not be applied or have been applied to VTC. Otherwise enter the number of cycles.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(TYPICAL VALUES: 3 is the BV default or 0 if performed on FMR instead)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leave blank or set 0 if THP should not have been performed on FMR. Otherwise, enter the number of cycles that should have been used.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(TYPICAL VALUES: 2 is the BV default or 0 if performing on VTC instead)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -373,8 +406,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E22" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E21"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -673,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,7 +723,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -707,13 +740,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -728,7 +761,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -740,13 +773,13 @@
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -761,17 +794,17 @@
     </row>
     <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -780,43 +813,43 @@
         <v>11</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -828,19 +861,19 @@
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6">
         <v>8</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -850,139 +883,129 @@
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="6" t="b">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="6">
-        <v>2</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C14" s="6"/>
       <c r="D14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C15" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="6">
-        <v>6</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>29</v>
-      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="5" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="C19" s="7"/>
       <c r="D19" s="5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
@@ -1046,13 +1069,6 @@
       <c r="C31" s="6"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
generate first set of prt too
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Value</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>E:\Guy\PRTs</t>
-  </si>
-  <si>
-    <t>Can include wildcard (*). Will replace [P#], [R#], and/or [PID]. If numbers are forced to a min number of digits (e.g., forcing 2-digits yields 02 instead of 2), state the number of digits after the #-sign. For example, [R#2] will insert a 2-digit run number.</t>
   </si>
   <si>
     <t>PAR[P#2]_RUN[R#2]*.prt</t>
@@ -312,6 +309,63 @@
       </rPr>
       <t>(TYPICAL VALUES: 6 or 8)</t>
     </r>
+  </si>
+  <si>
+    <t>Predictors</t>
+  </si>
+  <si>
+    <t>Names of predictor sets</t>
+  </si>
+  <si>
+    <t>Can include wildcard (*). Will replace [P#], [R#], [PID], and [PRED_SET]. If numbers are forced to a min number of digits (e.g., forcing 2-digits yields 02 instead of 2), state the number of digits after the #-sign. For example, [R#2] will insert a 2-digit run number.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">If there are multiple sets of predictors, state names of the sets here to replace [PRED_SET] below. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The first set will be linked to VTCs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Leave blank if not using [PRED_SET] in Naming (i.e., if there is only one set of predictors).</t>
+    </r>
+  </si>
+  <si>
+    <t>PRT.SETS</t>
   </si>
 </sst>
 </file>
@@ -433,8 +487,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E26"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -733,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,13 +854,13 @@
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -819,257 +873,255 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>44</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>60</v>
-      </c>
+      <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="6">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="6">
-        <v>1000</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C13" s="6">
-        <v>487</v>
+        <v>8</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6">
+        <v>487</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="6">
         <v>2</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5" t="s">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C20" s="6">
         <v>6</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C22" s="6"/>
       <c r="D22" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="D23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="6" t="b">
-        <v>1</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="5" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,11 +1132,21 @@
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="A26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
@@ -1141,6 +1203,20 @@
       <c r="C34" s="6"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
supports sets of PRT to generate sets of SDM/MDM
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -314,6 +314,18 @@
     <t>Can include wildcard (*). Will replace [P#], [R#], [PID], and [PRED_SET]. If numbers are forced to a min number of digits (e.g., forcing 2-digits yields 02 instead of 2), state the number of digits after the #-sign. For example, [R#2] will insert a 2-digit run number.</t>
   </si>
   <si>
+    <t>PRT.SETS</t>
+  </si>
+  <si>
+    <t>C:\Users\kmstu\Documents\GitHub\GR_fMRI_Actiontopy-Somatotopy\Experiment\PRTs</t>
+  </si>
+  <si>
+    <t>first, action-type_involved-effector, action, involved-effector, body_visibility, viewpoint, environment, actor</t>
+  </si>
+  <si>
+    <t>PAR[P#2]_RUN[R#2]_*_[PRED_SET].prt</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -333,7 +345,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The first set will be linked to VTCs.</t>
+      <t>The first set will be linked to VTCs, but SDM/MDM will be generated for each set.</t>
     </r>
     <r>
       <rPr>
@@ -357,18 +369,6 @@
       </rPr>
       <t>Leave blank if not using [PRED_SET] in Naming (i.e., if there is only one set of predictors).</t>
     </r>
-  </si>
-  <si>
-    <t>PRT.SETS</t>
-  </si>
-  <si>
-    <t>C:\Users\kmstu\Documents\GitHub\GR_fMRI_Actiontopy-Somatotopy\Experiment\PRTs</t>
-  </si>
-  <si>
-    <t>first, action-type_involved-effector, action, involved-effector, body_visibility, viewpoint, environment, actor</t>
-  </si>
-  <si>
-    <t>PAR[P#2]_RUN[R#2]_*_[PRED_SET].prt</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +860,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>46</v>
@@ -876,7 +876,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>67</v>
       </c>
@@ -884,13 +884,13 @@
         <v>68</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -908,7 +908,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
added excel field PRT.NUM_POI
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Value</t>
   </si>
@@ -89,12 +89,6 @@
   </si>
   <si>
     <t>Exclusions</t>
-  </si>
-  <si>
-    <t>E:\Guy\Guy_Pilot_Aug2018</t>
-  </si>
-  <si>
-    <t>E:\Guy\Script_Output</t>
   </si>
   <si>
     <t>Temporal high pass filter number of cycles (if running after preprocessing on vtc)</t>
@@ -317,7 +311,19 @@
     <t>PRT.SETS</t>
   </si>
   <si>
-    <t>C:\Users\kmstu\Documents\GitHub\GR_fMRI_Actiontopy-Somatotopy\Experiment\PRTs</t>
+    <t>C:\Users\kstubbs4\Documents\GitHub\GR_fMRI_Actiontopy-Somatotopy\Experiment\PRTs</t>
+  </si>
+  <si>
+    <t>D:\Users\kstubbs4\Guy\Guy_Pilot_Aug2018</t>
+  </si>
+  <si>
+    <t>D:\Users\kstubbs4\Guy\Guy_Pilot_Aug2018\Script_Output</t>
+  </si>
+  <si>
+    <t>PAR[P#2]_RUN[R#2]_*.prt</t>
+  </si>
+  <si>
+    <t>Number of predictors of interest</t>
   </si>
   <si>
     <r>
@@ -339,8 +345,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>The first set will be linked to VTCs, but SDM/MDM will be generated for each set.</t>
-    </r>
+      <t>The first set will be linked to VTCs, but SDM/MDM will be generated for each set. Leave blank if there is only one set.</t>
+    </r>
+  </si>
+  <si>
+    <t>PRT.NUM_POI</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -349,8 +360,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
+      <t>The first x-many predictors in the PRTs will be treated as predictors of interest.</t>
     </r>
     <r>
       <rPr>
@@ -361,14 +371,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Leave blank if not using [PRED_SET] in Naming (i.e., if there is only one set of predictors).</t>
-    </r>
-  </si>
-  <si>
-    <t>first, action-type_involved-effector, action-type, action, involved-effector, body_visibility, viewpoint, environment, actor</t>
-  </si>
-  <si>
-    <t>PAR[P#2]_RUN[R#2]_*_2018_[PRED_SET].prt</t>
+      <t xml:space="preserve">
+If left blank, then all predicors (except motion) will be predictors of interest.
+If using multiple predictor sets, separate with commas.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Example: If there are 3 sets of predictors when "10, 20, 30" will result in 10 POI in the first set, 20 in the second set, and 30 in the third set. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -490,8 +507,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E27"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -546,7 +563,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,7 +598,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -790,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -839,13 +856,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -857,13 +874,13 @@
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -876,73 +893,69 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C10" s="6"/>
       <c r="D10" s="5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,214 +964,222 @@
         <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="B12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="6">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1000</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="6">
-        <v>487</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="6">
+        <v>487</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="6" t="b">
+      <c r="E16" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="D17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="B19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="6">
         <v>2</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="6"/>
       <c r="D19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C21" s="6">
         <v>6</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="D21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="C25" s="7"/>
+      <c r="D25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="6" t="b">
+      <c r="C27" s="6" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -1222,6 +1243,13 @@
       <c r="C36" s="6"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
now supports variable PRT POI
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -372,7 +372,7 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-If left blank, then all predicors (except motion) will be predictors of interest.
+If left blank or set to &lt;1, then all predicors (except motion) will be predictors of interest.
 If using multiple predictor sets, separate with commas.
 </t>
     </r>
@@ -908,7 +908,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
supports MATLAB colon notation
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -61,9 +61,6 @@
     <t>EXCLUDE.PAR</t>
   </si>
   <si>
-    <t>Separate with commas. Spaces will be ignored. Example: "7, 8, 9, 10"</t>
-  </si>
-  <si>
     <t>EXCLUDE.PARRUN</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
   </si>
   <si>
     <t>If some participants have more runs, put the max number of runs unless you want to exclude those runs. Run with numbers greater than this value are completely ignored.</t>
-  </si>
-  <si>
-    <t>Separate with commas. Spaces will be ignored. Can use participant numbers (e.g., "1, 2") or IDs (e.g., "P1, P2" or "P01, P02" or "AB12, CD23")</t>
   </si>
   <si>
     <t>Separate with commas. Spaces will be ignored. Format as P#-R#. Example: "1-1, 1-2" (excludes runs 1 and 2 of particpant 1).</t>
@@ -386,6 +380,12 @@
       </rPr>
       <t xml:space="preserve">Example: If there are 3 sets of predictors when "10, 20, 30" will result in 10 POI in the first set, 20 in the second set, and 30 in the third set. </t>
     </r>
+  </si>
+  <si>
+    <t>Separate with commas. Spaces will be ignored. Can use participant numbers (e.g., "1, 2") or IDs (e.g., "P1, P2" or "P01, P02" or "AB12, CD23"). Can use MATLAB's colon notatation (e.g., "1, 3:10" excludes 1 and 3-through-10).</t>
+  </si>
+  <si>
+    <t>Separate with commas. Spaces will be ignored. Can use MATLAB's colon notatation (e.g., "7, 10:12" excludes 7 and 10-through-12).</t>
   </si>
 </sst>
 </file>
@@ -809,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -841,13 +841,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
@@ -862,7 +862,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -874,13 +874,13 @@
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -895,30 +895,30 @@
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -930,62 +930,62 @@
     </row>
     <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -997,64 +997,64 @@
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="6">
         <v>8</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6">
         <v>1000</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6">
         <v>487</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" s="6" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,32 +1066,32 @@
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>12</v>
@@ -1116,45 +1116,45 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="5" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1166,19 +1166,19 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="C27" s="6" t="b">
         <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added option for absolute filepath in mdm + text when complete vtc preprocess
</commit_message>
<xml_diff>
--- a/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
+++ b/Post-Preprocessing/BV20_PostPreprocessing_and_QualityChecks_EXAMPLE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Value</t>
   </si>
@@ -386,6 +386,18 @@
   </si>
   <si>
     <t>Separate with commas. Spaces will be ignored. Can use MATLAB's colon notatation (e.g., "7, 10:12" excludes 7 and 10-through-12).</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>Old BV requires absolute paths, but relative paths are more flexible (can move the directory, use on another computer, etc).</t>
+  </si>
+  <si>
+    <t>MDM.PATH_ABS</t>
+  </si>
+  <si>
+    <t>Use absolute paths in multi-participant MDMs</t>
   </si>
 </sst>
 </file>
@@ -507,8 +519,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E29"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Category" dataDxfId="4"/>
     <tableColumn id="5" name="Description" dataDxfId="3"/>
@@ -809,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,12 +1200,22 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>

</xml_diff>